<commit_message>
update with new commands
</commit_message>
<xml_diff>
--- a/docs/ChorusAPI.xlsx
+++ b/docs/ChorusAPI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="136">
   <si>
     <t>Request</t>
   </si>
@@ -924,6 +924,45 @@
   </si>
   <si>
     <t>As part of Bulk Device State request</t>
+  </si>
+  <si>
+    <t>Get LiPo Voltage</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>R*Y\n -&gt; S1Y00D5\n</t>
+  </si>
+  <si>
+    <t>Reading from analog voltage pin (2 bytes). Response comes only from nodes that have LiPo monitoring.</t>
+  </si>
+  <si>
+    <t>Get single RSSI reading</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Current RSSI Value (2 bytes)</t>
+  </si>
+  <si>
+    <t>R0E\n -&gt; S0S0111\n</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Set RSSI Monitor interval</t>
+  </si>
+  <si>
+    <t>RSSI monitor interval to set (2 bytes). Values are measured in ~0.1ms intervals. e.g. value of 1000 (decimal) gives 100ms. Min allowed value is 0xA.</t>
+  </si>
+  <si>
+    <t>RSSI monitor interval (2 bytes) (see request description)</t>
+  </si>
+  <si>
+    <t>R1d0001\n -&gt; S1d000A\n</t>
   </si>
 </sst>
 </file>
@@ -1343,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="31.5" customHeight="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1924,135 +1963,199 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>50</v>
+    <row r="28" spans="1:7" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="B28" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>52</v>
+        <v>131</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+    <row r="33" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="4">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="34" spans="1:7" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+    <row r="35" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+    <row r="36" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>79</v>
       </c>
     </row>
+    <row r="37" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add voltage conversion formula
</commit_message>
<xml_diff>
--- a/docs/ChorusAPI.xlsx
+++ b/docs/ChorusAPI.xlsx
@@ -510,9 +510,6 @@
     <t>API version</t>
   </si>
   <si>
-    <t>Reading from analog voltage pin. Response comes only from nodes that have LiPo attached.</t>
-  </si>
-  <si>
     <t>Was node configured (i.e. any "set" command was performed on this node since start). 
 1 = configured 
 0 = not configured 
@@ -575,12 +572,30 @@
     <t>Wait for Min Lap time before detecting first lap in a race mode. 1 = wait 
 0 = disregard Min Lap Time for first lap, report as soon as detected)</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reading from analog voltage pin. Response comes only from nodes that have LiPo attached.
+Conversion to actual voltage:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>V = VRead*((R1+R2)/R2)*(Varduino/1024)
+or, with constants computed :
+V = Vread * 55 / 1024</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,6 +624,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FF24292E"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -995,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="31.5" customHeight="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1194,7 +1215,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="114" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1208,7 +1229,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>68</v>
@@ -1231,7 +1252,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>69</v>
@@ -1277,7 +1298,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>69</v>
@@ -1300,7 +1321,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>72</v>
@@ -1311,7 +1332,7 @@
     </row>
     <row r="14" spans="1:7" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="4">
         <v>4</v>
@@ -1323,7 +1344,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>69</v>
@@ -1334,7 +1355,7 @@
     </row>
     <row r="15" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="4">
         <v>4</v>
@@ -1346,7 +1367,7 @@
         <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>69</v>
@@ -1357,7 +1378,7 @@
     </row>
     <row r="16" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="4">
         <v>4</v>
@@ -1369,7 +1390,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>68</v>
@@ -1380,7 +1401,7 @@
     </row>
     <row r="17" spans="1:7" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="4">
         <v>4</v>
@@ -1392,7 +1413,7 @@
         <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>68</v>
@@ -1415,7 +1436,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>69</v>
@@ -1461,7 +1482,7 @@
         <v>16</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>68</v>
@@ -1484,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>69</v>
@@ -1593,25 +1614,25 @@
     <row r="32" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update support for power-down mode in android app; update API version and docs
</commit_message>
<xml_diff>
--- a/docs/ChorusAPI.xlsx
+++ b/docs/ChorusAPI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="115">
   <si>
     <t>Request</t>
   </si>
@@ -628,6 +628,21 @@
   </si>
   <si>
     <t>whatever format is used for debugging, even plain text</t>
+  </si>
+  <si>
+    <t>Activate/Deactivate Rx module</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Rx Module Power State
+1 = On, 0 = Off
+Can be used to turn off unused module to decrease overall power consumption</t>
+  </si>
+  <si>
+    <t>get: R0A\n -&gt; S0A0\n
+set: R0A0\n -&gt; S0A0\n</t>
   </si>
 </sst>
 </file>
@@ -802,17 +817,17 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="31.5" customHeight="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1250,7 +1265,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="4">
@@ -1273,7 +1288,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="4">
         <v>5</v>
       </c>
@@ -1283,13 +1298,13 @@
       <c r="D8" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1661,107 +1676,127 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="4">
+        <v>6</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B26" s="4">
         <v>5</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+    <row r="27" spans="1:7" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="129" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="129" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B28" s="4">
         <v>1</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="5"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="8"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="5"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="F30" s="3"/>
+      <c r="D30" s="8"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="6"/>
+    </row>
     <row r="32" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="5:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="5:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="5:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="5:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E36"/>
-    </row>
+    <row r="36" spans="5:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="5:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E37"/>
     </row>
@@ -1821,6 +1856,9 @@
     </row>
     <row r="56" spans="5:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E56"/>
+    </row>
+    <row r="57" spans="5:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>